<commit_message>
Update final: Config Render, Automatizacion 7AM y Glosario Teorico
</commit_message>
<xml_diff>
--- a/data/reporte_fenomenos_20260121.xlsx
+++ b/data/reporte_fenomenos_20260121.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,7 +493,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -531,19 +531,19 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>DIRECCIÓN NACIONAL DE VIALIDADResolución 69/2026RESOL-2026-69-APN-DNV#MEC</t>
+          <t>PROCEDIMIENTOS ADMINISTRATIVOSDecreto 25/2026DECTO-2026-25-APN-PTE - Recházase recurso.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337599/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337566/20260120</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -581,19 +581,19 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>ENTE NACIONAL REGULADOR DEL GASResolución 15/2026RESOL-2026-15-APN-DIRECTORIO#ENARGAS</t>
+          <t>PRESUPUESTODecisión Administrativa 1/2026DA-2026-1-APN-JGM - Presupuesto General de la Administración Nacional para el Ejercicio 2026. Distributivo.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337600/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337567/20260120</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -631,19 +631,19 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>MINISTERIO DE CAPITAL HUMANO - SECRETARÍA DE TRABAJO, EMPLEO Y SEGURIDAD SOCIALResolución 79/2026RESOL-2026-79-APN-STEYSS#MCH</t>
+          <t>ADMINISTRACIÓN NACIONAL DE AVIACIÓN CIVILResolución 35/2026RESOL-2026-35-APN-ANAC#MEC</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337601/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337568/20260120</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -681,19 +681,19 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>MINISTERIO DE ECONOMÍA - SECRETARÍA DE INDUSTRIA Y COMERCIOResolución 20/2026RESOL-2026-20-APN-SIYC#MEC</t>
+          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERO - DIRECCIÓN GENERAL DE ADUANASResolución 8/2026RESOL-2026-8-E-ARCA-DGADUA</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337602/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337569/20260120</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -731,19 +731,19 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>MINISTERIO DE ECONOMÍA - SECRETARÍA DE OBRAS PÚBLICASResolución 9/2026RESOL-2026-9-APN-SOP#MEC</t>
+          <t>INSTITUTO NACIONAL DE CINE Y ARTES AUDIOVISUALESResolución 9/2026RESOL-2026-9-APN-INCAA#SC</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337603/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337570/20260120</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -781,19 +781,19 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>MINISTERIO DE ECONOMÍA - SECRETARÍA DE OBRAS PÚBLICASResolución 11/2026RESOL-2026-11-APN-SOP#MEC</t>
+          <t>INSTITUTO NACIONAL DE LA YERBA MATEResolución 2/2026</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337604/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337571/20260120</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -831,19 +831,19 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>MINISTERIO DE SEGURIDAD NACIONALResolución 47/2026RESOL-2026-47-APN-MSG</t>
+          <t>JEFATURA DE GABINETE DE MINISTROS - SECRETARÍA DE COORDINACIÓN LEGAL Y ADMINISTRATIVAResolución 6/2026RESOL-2026-6-APN-SCLYA#JGM</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337605/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337572/20260120</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -881,19 +881,19 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANEROResolución General 5816/2026RESOG-2026-5816-E-ARCA-ARCA - Procedimiento. Sociedades de Garantía Recíproca (S.G.R.). Socios Protectores. Régimen de información. Resolución General...</t>
+          <t>MINISTERIO DE ECONOMÍA - SECRETARÍA DE ENERGÍAResolución 15/2026RESOL-2026-15-APN-SE#MEC</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337606/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337573/20260120</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -931,19 +931,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANEROResolución General 5817/2026RESOG-2026-5817-E-ARCA-ARCA - Seguridad Social. Decreto N° 394/23 y sus modificatorios. Beneficio a Microempresas. Pago a cuenta de contribuciones pat...</t>
+          <t>MINISTERIO DE ECONOMÍA - SECRETARÍA DE INDUSTRIA Y COMERCIOResolución 19/2026RESOL-2026-19-APN-SIYC#MEC</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337607/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337574/20260120</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -981,19 +981,19 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>AGENCIA DE PLANIFICACIÓNResolución Sintetizada 1/2026</t>
+          <t>MINISTERIO DE SALUDResolución 238/2026RESOL-2026-238-APN-MS</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337608/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337575/20260120</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1031,19 +1031,19 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>ENTE NACIONAL REGULADOR DE LA ELECTRICIDADResolución Sintetizada 13/2026</t>
+          <t>MINISTERIO DE SEGURIDAD NACIONALResolución 40/2026RESOL-2026-40-APN-MSG</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337609/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337576/20260120</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1081,19 +1081,19 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>ADMINISTRACIÓN NACIONAL DE MEDICAMENTOS, ALIMENTOS Y TECNOLOGÍA MÉDICADisposición 63/2026DI-2026-63-APN-ANMAT#MS</t>
+          <t>MINISTERIO DE SEGURIDAD NACIONAL Y MINISTERIO DE RELACIONES EXTERIORES, COMERCIO INTERNACIONAL Y CULTOResolución Conjunta 1/2026RESFC-2026-1-APN-MSG</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337610/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337577/20260120</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1103,47 +1103,47 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>No identificado</t>
+          <t>Tarifas Servicios Públicos</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>Legal(30) + Discrec(30) + Certeza Muy Alta(40) = 100%</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Indeterminado</t>
+          <t>Usuarios / Población</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Indeterminado</t>
+          <t>Empresas Concesionarias</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>No detectado</t>
+          <t>Aumento de tarifa o subsidio cruzado</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>ADMINISTRACIÓN NACIONAL DE MEDICAMENTOS, ALIMENTOS Y TECNOLOGÍA MÉDICADisposición 66/2026DI-2026-66-APN-ANMAT#MS</t>
+          <t>ENTE REGULADOR DE AGUA Y SANEAMIENTOResolución Sintetizada 1/2026</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337611/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337578/20260120</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1181,19 +1181,19 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>ADMINISTRACIÓN NACIONAL DE MEDICAMENTOS, ALIMENTOS Y TECNOLOGÍA MÉDICADisposición 68/2026DI-2026-68-APN-ANMAT#MS</t>
+          <t>SUPERINTENDENCIA DE SEGUROS DE LA NACIÓNResolución Sintetizada 14/2026</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337612/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337579/20260120</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1231,19 +1231,19 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERODisposición 5/2026DI-2026-5-E-ARCA-ARCA</t>
+          <t>ADMINISTRACIÓN NACIONAL DE MEDICAMENTOS, ALIMENTOS Y TECNOLOGÍA MÉDICADisposición 47/2026DI-2026-47-APN-ANMAT#MS</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337613/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337580/20260120</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1281,19 +1281,19 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERO - ADUANA OBERÁDisposición 6/2026DI-2026-6-E-ARCA-ADOBER#SDGOAI</t>
+          <t>ADMINISTRACIÓN NACIONAL DE MEDICAMENTOS, ALIMENTOS Y TECNOLOGÍA MÉDICADisposición 72/2026DI-2026-72-APN-ANMAT#MS</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337614/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337581/20260120</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1331,19 +1331,19 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>ENTE NACIONAL DE COMUNICACIONESDisposición Sintetizada 235/2026</t>
+          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERO - DIRECCIÓN REGIONAL SALTADisposición 3/2026DI-2026-3-E-ARCA-DIRSAL#SDGOPII</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337615/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337582/20260120</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1381,19 +1381,19 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>ENTE NACIONAL DE COMUNICACIONESDisposición Sintetizada 1328/2026</t>
+          <t>AGENCIA NACIONAL DE SEGURIDAD VIALDisposición 10/2026DI-2026-10-APN-ANSV#MEC</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337616/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337583/20260120</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1431,19 +1431,19 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>ENTE NACIONAL DE COMUNICACIONESDisposición Sintetizada 1359/2026</t>
+          <t>AGENCIA NACIONAL DE SEGURIDAD VIALDisposición 11/2026DI-2026-11-APN-ANSV#MEC</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337617/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337584/20260120</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1481,19 +1481,19 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>ENTE NACIONAL DE COMUNICACIONESDisposición Sintetizada 1814/2026</t>
+          <t>MINISTERIO DE ECONOMÍA - SUBSECRETARÍA DE TRANSICIÓN Y PLANEAMIENTO ENERGÉTICODisposición 1/2026DI-2026-1-APN-SSTYPE#MEC</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337618/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337585/20260120</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1531,19 +1531,19 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>BANCO DE LA NACIÓN ARGENTINAAviso Oficial</t>
+          <t>MINISTERIO DE ECONOMÍA - SUBSECRETARÍA DE TRANSICIÓN Y PLANEAMIENTO ENERGÉTICODisposición 2/2026DI-2026-2-APN-SSTYPE#MEC</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337619/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337586/20260120</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1581,19 +1581,19 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>BANCO CENTRAL DE LA REPÚBLICA ARGENTINAComunicación "B" 13110/2026</t>
+          <t>PREFECTURA NAVAL ARGENTINADisposición 39/2026DISFC-2026-39-APN-PNA#MSG</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337620/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337587/20260120</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1631,19 +1631,19 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERO - DIRECCIÓN ADUANA DE BUENOS AIRESAviso Oficial</t>
+          <t>ENTE NACIONAL DE COMUNICACIONESDisposición Sintetizada 1326/2026</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337621/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337588/20260120</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1681,19 +1681,19 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>INSTITUTO NACIONAL DE ASOCIATIVISMO Y ECONOMÍA SOCIALAviso Oficial</t>
+          <t>ENTE NACIONAL DE COMUNICACIONESDisposición Sintetizada 1329/2026</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337622/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337589/20260120</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1731,19 +1731,19 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>INSTITUTO NACIONAL DE ASOCIATIVISMO Y ECONOMÍA SOCIALAviso Oficial</t>
+          <t>ENTE NACIONAL DE COMUNICACIONESDisposición Sintetizada 1489/2026</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337623/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337590/20260120</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1781,19 +1781,19 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>INSTITUTO NACIONAL DE ASOCIATIVISMO Y ECONOMÍA SOCIALAviso Oficial</t>
+          <t>BANCO DE LA NACIÓN ARGENTINAAviso Oficial</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337624/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337591/20260120</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1831,19 +1831,19 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>INSTITUTO NACIONAL DE ASOCIATIVISMO Y ECONOMÍA SOCIALAviso Oficial</t>
+          <t>BANCO CENTRAL DE LA REPÚBLICA ARGENTINAAviso Oficial</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337625/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337592/20260120</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1886,14 +1886,14 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337626/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337593/20260120</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1931,19 +1931,19 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>BANCO CENTRAL DE LA REPÚBLICA ARGENTINAAviso Oficial</t>
+          <t>INSTITUTO NACIONAL DE SEMILLASAviso Oficial</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337627/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337594/20260120</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1981,19 +1981,19 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>BANCO CENTRAL DE LA REPÚBLICA ARGENTINAAviso Oficial</t>
+          <t>MINISTERIO DE ECONOMÍA - SUBSECRETARÍA DE ENERGÍA ELÉCTRICAAviso Oficial</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337628/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337595/20260120</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2031,24 +2031,24 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>INSTITUTO NACIONAL DE ASOCIATIVISMO Y ECONOMÍA SOCIALAviso Oficial</t>
+          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANEROAviso Oficial</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337629/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337596/20260120</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>tercera</t>
+          <t>primera</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2081,69 +2081,69 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>POLICÍA FEDERAL ARGENTINALicitación Pública 32/2025</t>
+          <t>BANCO CENTRAL DE LA REPÚBLICA ARGENTINAAviso Oficial</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407023/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337597/20260120</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>tercera</t>
+          <t>primera</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>No identificado</t>
+          <t>Servicios Privados (Salud/Educación)</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>Legal(30) + Discrec(30) + Certeza Alta(30) = 90%</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Indeterminado</t>
+          <t>Salario de los Trabajadores</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Indeterminado</t>
+          <t>Empresas de Salud/Educación</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>No detectado</t>
+          <t>Autorización de aumento por encima de inflación</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>BANCO CENTRAL DE LA REPÚBLICA ARGENTINALicitación Pública 58/25</t>
+          <t>SUPERINTENDENCIA DE SERVICIOS DE SALUDAviso Oficial</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407024/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/primera/337598/20260120</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2181,19 +2181,19 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>AGUA Y SANEAMIENTOS ARGENTINOS S.A.Licitación Pública Nacional 64765/2026</t>
+          <t>MINISTERIO DE SEGURIDAD NACIONALLicitación Pública 0028/2025</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407025/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406958/20260120</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2231,19 +2231,19 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0013/2026</t>
+          <t>COMISIÓN NACIONAL DE ENERGÍA ATÓMICALicitación Pública 0051/2025</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407026/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406959/20260120</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2281,19 +2281,19 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>GENDARMERÍA NACIONAL ARGENTINALicitación Pública 69/2025</t>
+          <t>EJÉRCITO ARGENTINOLicitación Pública 1223/2025</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407027/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406960/20260120</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2331,19 +2331,19 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>MINISTERIO DE SEGURIDAD NACIONALLicitación Pública 0028/2025</t>
+          <t>HONORABLE CÁMARA DE DIPUTADOS DE LA NACIÓNLicitación Pública 21/2025</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407028/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406961/20260120</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2381,19 +2381,19 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0011/2026</t>
+          <t>COMISIÓN NACIONAL DE ENERGÍA ATÓMICALicitación Pública 60/2025</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407029/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406962/20260120</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2431,19 +2431,19 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0012/2026</t>
+          <t>BELGRANO CARGAS Y LOGÍSTICA S.A.Concurso Privado BCYL0010/2026</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407030/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406963/20260120</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2481,19 +2481,19 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0016/2026</t>
+          <t>BELGRANO CARGAS Y LOGÍSTICA S.A.Concurso Privado BCYL0012/2026</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407031/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406964/20260120</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2531,19 +2531,19 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0018/2026</t>
+          <t>AGUA Y SANEAMIENTOS ARGENTINOS S.A.Licitación Pública Nacional 65020/2026</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407032/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406965/20260120</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2581,19 +2581,19 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0029/2026</t>
+          <t>JEFATURA DE GABINETE DE MINISTROSLicitación Pública 33/2025</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407033/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406966/20260120</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2631,19 +2631,19 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>COMISIÓN NACIONAL DE ENERGÍA ATÓMICALicitación Pública 0051/2025</t>
+          <t>POLICÍA FEDERAL ARGENTINALicitación Pública 0001/2026</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407034/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406967/20260120</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2681,19 +2681,19 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>CONSEJO NACIONAL DE INVESTIGACIONES CIENTÍFICAS Y TÉCNICASLicitación 01/2026</t>
+          <t>HOSPITAL DE ALTA COMPLEJIDAD EL CALAFATELicitación Pública 0002-2026</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407035/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406968/20260120</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2731,19 +2731,19 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 1147/2025</t>
+          <t>INSTITUTO NACIONAL DE INVESTIGACIÓN Y DESARROLLO PESQUEROConcurso Público 0009/2025</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407036/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406969/20260120</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2781,19 +2781,19 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 1223/2025</t>
+          <t>POLICÍA FEDERAL ARGENTINALicitación Pública 0099/2025</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407037/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406970/20260120</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2831,19 +2831,19 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>CASA DE MONEDA SOCIEDAD ANÓNIMA UNIPERSONALLicitación Pública 966</t>
+          <t>POLICÍA FEDERAL ARGENTINALicitación Pública 0104/2025</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407038/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406971/20260120</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2881,19 +2881,19 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>CASA DE MONEDA SOCIEDAD ANÓNIMA UNIPERSONALLicitación Pública 971/2026</t>
+          <t>EJÉRCITO ARGENTINOLicitación Pública 1214/2025</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407039/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406972/20260120</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2931,19 +2931,19 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>CASA DE MONEDA SOCIEDAD ANÓNIMA UNIPERSONALLicitación Pública 972</t>
+          <t>EJÉRCITO ARGENTINOLicitación Pública 1215/2025</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407040/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406973/20260120</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2981,19 +2981,19 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>BELGRANO CARGAS Y LOGÍSTICA S.A.Concurso Privado BCYL0010/2026</t>
+          <t>EJÉRCITO ARGENTINOLicitación Pública 1226/2025</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407041/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406974/20260120</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -3031,19 +3031,19 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>BELGRANO CARGAS Y LOGÍSTICA S.A.Concurso Privado BCYL0012/2026</t>
+          <t>BELGRANO CARGAS Y LOGÍSTICA S.A.Concurso Privado BCYL0011/2026</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407042/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406975/20260120</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -3081,19 +3081,19 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>AGUA Y SANEAMIENTOS ARGENTINOS S.A.Licitación Pública Nacional 64534/2026</t>
+          <t>UNIVERSIDAD NACIONAL DE LA PAMPALicitación Pública 01/2026</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407043/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406976/20260120</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -3131,19 +3131,20 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0015/2026</t>
+          <t>UNIVERSIDAD DE BUENOS AIRES - 
+DIRECCIÓN GENERAL DE PLANIFICACIÓN Y GESTIÓN DE CONTRATACIONESLicitación Pública 01/2026</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407044/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406977/20260120</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -3181,19 +3182,20 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>POLICÍA FEDERAL ARGENTINALicitación Pública 0001/2026</t>
+          <t>UNIVERSIDAD NACIONAL DE LA PLATA - 
+SECRETARÍA DE PLANEAMIENTO, OBRAS Y SERVICIOSLicitación Pública 01/26</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407045/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406978/20260120</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -3231,19 +3233,19 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>HOSPITAL DE ALTA COMPLEJIDAD EL CALAFATELicitación Pública 0002-2026</t>
+          <t>PROVINCIA DEL CHUBUT  - MUNICIPALIDAD DE RÍO MAYOLicitación Pública 01/2026 – M.R.M.</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407046/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406979/20260120</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -3281,19 +3283,20 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>POLICÍA FEDERAL ARGENTINALicitación Pública 0099/2025</t>
+          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERO - 
+DIRECCIÓN REGIONAL ADUANERA NORESTELicitación Pública 04/2026</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407047/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406980/20260120</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -3331,19 +3334,19 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>POLICÍA FEDERAL ARGENTINALicitación Pública 0104/2025</t>
+          <t>ADMINISTRACIÓN NACIONAL DE LA SEGURIDAD SOCIALLicitación Pública PROCESO COMPR.AR 63-0074-LPU25</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406997/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406981/20260120</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -3381,19 +3384,19 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0955/2025</t>
+          <t>MINISTERIO DE ECONOMÍALicitación Pública 0026/2025</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406998/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406982/20260120</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -3431,19 +3434,19 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 1226/2025</t>
+          <t>SECRETARÍA LEGAL Y TÉCNICALicitación Pública 3/2025</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406999/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406983/20260120</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -3481,19 +3484,19 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>BELGRANO CARGAS Y LOGÍSTICA S.A.Concurso Privado BCYL0011/2026</t>
+          <t>COMISIÓN NACIONAL DE ENERGÍA ATÓMICALicitación Pública 53/2025</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407000/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406984/20260120</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -3531,19 +3534,19 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0010/2026</t>
+          <t>AGUA Y SANEAMIENTOS ARGENTINOS S.A.Licitación Pública Nacional 64888/2026</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407001/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406985/20260120</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -3581,19 +3584,19 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0014/2026</t>
+          <t>AGUA Y SANEAMIENTOS ARGENTINOS S.A.Licitación Pública Nacional 64950/2026</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407002/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406986/20260120</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -3631,19 +3634,19 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>UNIVERSIDAD NACIONAL DE LA PAMPALicitación Pública 01/2026</t>
+          <t>GOBIERNO DE LA PROVINCIA DE RÍO NEGRO - SECRETARÍA DE HIDROCARBUROS - SECRETARÍA DE ESTADO DE ENERGÍA Y AMBIENTEConcurso Público Nacional e Internacional 02/25</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407003/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406987/20260120</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -3681,20 +3684,19 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>UNIVERSIDAD DE BUENOS AIRES - 
-DIRECCIÓN GENERAL DE PLANIFICACIÓN Y GESTIÓN DE CONTRATACIONESLicitación Pública 01/2026</t>
+          <t>AGENCIA DE ADMINISTRACIÓN DE BIENES DEL ESTADOSubasta Pública 392-0091-SPU25</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407004/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406988/20260120</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -3732,20 +3734,19 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>UNIVERSIDAD NACIONAL DE LA PLATA - 
-SECRETARÍA DE PLANEAMIENTO, OBRAS Y SERVICIOSLicitación Pública 01/26</t>
+          <t>AGENCIA DE ADMINISTRACIÓN DE BIENES DEL ESTADOSubasta Pública 392-0094-SPU25</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407005/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406989/20260120</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -3783,19 +3784,20 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>PROVINCIA DEL CHUBUT  - MUNICIPALIDAD DE RÍO MAYOLicitación Pública 01/2026 – M.R.M.</t>
+          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERO - 
+DIRECCIÓN REGIONAL ADUANERA CENTRALLicitación Pública 20/25</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407006/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406990/20260120</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -3833,20 +3835,19 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERO - 
-DIRECCIÓN REGIONAL ADUANERA NORESTELicitación Pública 04/2026</t>
+          <t>COMISIÓN NACIONAL DE ENERGÍA ATÓMICAConcurso Público 0004/2025</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407007/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406991/20260120</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -3884,20 +3885,19 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERO  - 
-DIRECCIÓN REGIONAL ADUANERA AUSTRALLicitación Pública 28/25</t>
+          <t>SERVICIO PENITENCIARIO FEDERALLicitación Pública 0025/2025</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407008/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406992/20260120</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -3935,19 +3935,19 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0009/2026</t>
+          <t>EJÉRCITO ARGENTINOLicitación Pública 1170/2025</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407009/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406993/20260120</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -3985,19 +3985,19 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0017/2026</t>
+          <t>EJÉRCITO ARGENTINOLicitación Pública 1172/2025</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407010/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406994/20260120</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -4035,19 +4035,19 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0028/2026</t>
+          <t>EJÉRCITO ARGENTINOLicitación Pública 1191/2025</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407011/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406995/20260120</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>20260121</t>
+          <t>20260120</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -4085,514 +4085,13 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0030/2026</t>
+          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERO - 
+DIRECCIÓN REGIONAL SURLicitación Pública 14/25</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407012/20260121</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>20260121</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>tercera</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>No identificado</t>
-        </is>
-      </c>
-      <c r="D74" t="n">
-        <v>0</v>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>No aplica</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>No detectado</t>
-        </is>
-      </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 0031/2026</t>
-        </is>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407013/20260121</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>20260121</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>tercera</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>No identificado</t>
-        </is>
-      </c>
-      <c r="D75" t="n">
-        <v>0</v>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>No aplica</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>No detectado</t>
-        </is>
-      </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERO - 
-DIRECCIÓN REGIONAL ADUANERA AUSTRALLicitación Pública 01/26</t>
-        </is>
-      </c>
-      <c r="J75" t="inlineStr">
-        <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407014/20260121</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>20260121</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>tercera</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>No identificado</t>
-        </is>
-      </c>
-      <c r="D76" t="n">
-        <v>0</v>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>No aplica</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>No detectado</t>
-        </is>
-      </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>NUCLEOELÉCTRICA ARGENTINA S.A.Licitación Pública</t>
-        </is>
-      </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407015/20260121</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>20260121</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>tercera</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>No identificado</t>
-        </is>
-      </c>
-      <c r="D77" t="n">
-        <v>0</v>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>No aplica</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>No detectado</t>
-        </is>
-      </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>DIRECCIÓN DE OBRA SOCIAL DEL SERVICIO PENITENCIARIO FEDERALSelección por Concurso SC-7-2025</t>
-        </is>
-      </c>
-      <c r="J77" t="inlineStr">
-        <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407016/20260121</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>20260121</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>tercera</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>No identificado</t>
-        </is>
-      </c>
-      <c r="D78" t="n">
-        <v>0</v>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>No aplica</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>No detectado</t>
-        </is>
-      </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>GOBIERNO DE LA PROVINCIA DE RÍO NEGRO - SECRETARÍA DE HIDROCARBUROS - SECRETARÍA DE ESTADO DE ENERGÍA Y AMBIENTEConcurso Público Nacional e Internacional 02/25</t>
-        </is>
-      </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407017/20260121</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>20260121</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>tercera</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>No identificado</t>
-        </is>
-      </c>
-      <c r="D79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>No aplica</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>No detectado</t>
-        </is>
-      </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>INSTITUTO NACIONAL DE SERVICIOS SOCIALES PARA JUBILADOS Y PENSIONADOSSubasta On Line con Base 3813</t>
-        </is>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407018/20260121</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>20260121</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>tercera</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>No identificado</t>
-        </is>
-      </c>
-      <c r="D80" t="n">
-        <v>0</v>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>No aplica</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>No detectado</t>
-        </is>
-      </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 1082/2025</t>
-        </is>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407019/20260121</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>20260121</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>tercera</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>No identificado</t>
-        </is>
-      </c>
-      <c r="D81" t="n">
-        <v>0</v>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>No aplica</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>No detectado</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 1087/2025</t>
-        </is>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407020/20260121</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>20260121</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>tercera</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>No identificado</t>
-        </is>
-      </c>
-      <c r="D82" t="n">
-        <v>0</v>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>No aplica</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Indeterminado</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>No detectado</t>
-        </is>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>EJÉRCITO ARGENTINOLicitación Pública 1089/2025</t>
-        </is>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407021/20260121</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>20260121</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>tercera</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Obra Pública / Contratos</t>
-        </is>
-      </c>
-      <c r="D83" t="n">
-        <v>85</v>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>Legal(30) + Discrec(30) + Certeza Media-Alta(25) = 85%</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>Contribuyentes (Impuestos Futuros)</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Empresas Contratistas</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Sobreprecios o continuación ineficiente</t>
-        </is>
-      </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>AGENCIA DE RECAUDACIÓN Y CONTROL ADUANERO  - 
-DIRECCIÓN REGIONAL ADUANERA NORESTEContratación Directa 82/25</t>
-        </is>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2407022/20260121</t>
+          <t>https://www.boletinoficial.gob.ar/detalleAviso/tercera/2406996/20260120</t>
         </is>
       </c>
     </row>

</xml_diff>